<commit_message>
Final changes for v5
</commit_message>
<xml_diff>
--- a/DataLoad/IndicatorMeasures.xlsx
+++ b/DataLoad/IndicatorMeasures.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\assal01\Documents\GitHub\Strategic-Alignment\DataLoad\"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3192" uniqueCount="1039">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3196" uniqueCount="1043">
   <si>
     <t>KPI</t>
   </si>
@@ -3141,6 +3141,18 @@
   </si>
   <si>
     <t>IM0458</t>
+  </si>
+  <si>
+    <t>Maintenance ==&gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t>Percent:</t>
+  </si>
+  <si>
+    <t>2014-Q4</t>
+  </si>
+  <si>
+    <t>PeriodToAdd</t>
   </si>
 </sst>
 </file>
@@ -3156,12 +3168,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -3176,8 +3194,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3482,10 +3502,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F524"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:N524"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3494,9 +3515,14 @@
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.5703125" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="12" max="12" width="1.85546875" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3512,8 +3538,23 @@
       <c r="E1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1041</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="N1" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>492</v>
       </c>
@@ -3533,7 +3574,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>492</v>
       </c>
@@ -3550,7 +3591,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>492</v>
       </c>
@@ -3567,7 +3608,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>492</v>
       </c>
@@ -3584,7 +3625,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>492</v>
       </c>
@@ -3601,7 +3642,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>492</v>
       </c>
@@ -3618,7 +3659,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>492</v>
       </c>
@@ -3635,7 +3676,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>492</v>
       </c>
@@ -3652,7 +3693,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>492</v>
       </c>
@@ -3669,7 +3710,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>492</v>
       </c>
@@ -3686,7 +3727,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>492</v>
       </c>
@@ -3703,7 +3744,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>492</v>
       </c>
@@ -3720,7 +3761,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>492</v>
       </c>
@@ -3737,7 +3778,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>492</v>
       </c>
@@ -3754,7 +3795,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>492</v>
       </c>
@@ -12492,6 +12533,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F277"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17297,6 +17339,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>